<commit_message>
YOUR UPDATED FILE COMMIT MESSAGE HERE
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>RuleSet</t>
   </si>
@@ -19,12 +19,6 @@
     <t>com.zubale.quest</t>
   </si>
   <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Quest</t>
-  </si>
-  <si>
     <t>Import</t>
   </si>
   <si>
@@ -37,7 +31,7 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>RuleTable RewardAmountNew</t>
+    <t>RuleTable RewardAmount</t>
   </si>
   <si>
     <t>CONDITION</t>
@@ -55,16 +49,16 @@
     <t>$quest.platform == "$param"</t>
   </si>
   <si>
-    <t>$quest.storeId == "$param"</t>
+    <t>$quest.storeId == "$1"</t>
   </si>
   <si>
     <t>$quest.distance $param</t>
   </si>
   <si>
-    <t>$quest.lines &lt;= $param</t>
-  </si>
-  <si>
-    <t>$quest.setRewardAmount(Float.parseFloat("$1"));</t>
+    <t>$quest.lines $param</t>
+  </si>
+  <si>
+    <t>$quest.setCalculate("$1");</t>
   </si>
   <si>
     <t>platform</t>
@@ -85,16 +79,52 @@
     <t>petco</t>
   </si>
   <si>
-    <t>&lt; 5</t>
-  </si>
-  <si>
-    <t>REWARD_AMOUNT_NEW</t>
+    <t>REWARD_AMOUNT</t>
   </si>
   <si>
     <t>walmart</t>
   </si>
   <si>
-    <t>&gt;=7</t>
+    <t>(35 + 5 * dist + 1 * lin)</t>
+  </si>
+  <si>
+    <t>chedraui</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>&lt;=8</t>
+  </si>
+  <si>
+    <t>&lt;=2</t>
+  </si>
+  <si>
+    <t>333, 444</t>
+  </si>
+  <si>
+    <t>&gt;=9</t>
+  </si>
+  <si>
+    <t>&gt;=3</t>
+  </si>
+  <si>
+    <t>666, 777, 888</t>
+  </si>
+  <si>
+    <t>&gt;=25</t>
+  </si>
+  <si>
+    <t>75 + (dist - 8) * 6.25</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>!=0</t>
+  </si>
+  <si>
+    <t>(75 + (25 - 8) * 6.25)</t>
   </si>
   <si>
     <t>general</t>
@@ -104,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -113,7 +143,7 @@
     <font>
       <b/>
       <sz val="8.0"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -125,12 +155,6 @@
     <font>
       <sz val="8.0"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8.0"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font/>
@@ -250,52 +274,52 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -304,23 +328,32 @@
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,210 +588,266 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="5"/>
+      <c r="B3" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="13"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="9" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="11" t="s">
+      <c r="B7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
+      <c r="F7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="8"/>
     </row>
     <row r="8">
-      <c r="A8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="15" t="s">
+      <c r="A8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="5"/>
+      <c r="C9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="8"/>
     </row>
     <row r="10">
-      <c r="A10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="15" t="s">
+      <c r="A10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="15" t="s">
+      <c r="B10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="C10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="8"/>
     </row>
     <row r="11">
-      <c r="A11" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="19" t="s">
+      <c r="A11" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="F11" s="22">
+        <v>25.0</v>
+      </c>
+      <c r="G11" s="8"/>
     </row>
     <row r="12">
       <c r="A12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="22">
-        <v>123.0</v>
-      </c>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="22">
-        <v>3.0</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="22">
-        <v>102.0</v>
-      </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13">
       <c r="A13" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="22">
-        <v>456.0</v>
-      </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="22">
-        <v>2.0</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>25</v>
+      <c r="D13" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>22</v>
       </c>
       <c r="F13" s="22">
-        <v>180.0</v>
-      </c>
-      <c r="G13" s="5"/>
+        <v>95.0</v>
+      </c>
+      <c r="G13" s="8"/>
     </row>
     <row r="14">
       <c r="A14" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="22">
+        <v>25</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="22">
+        <v>75.0</v>
+      </c>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="22">
         <v>789.0</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="22">
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="22">
         <v>150.0</v>
       </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15">
-      <c r="G15" s="5"/>
+      <c r="G17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A8:D8"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>